<commit_message>
Update gitignore, database file, and add click tracking patch
</commit_message>
<xml_diff>
--- a/database_ready_final (Marine Parade).xlsx
+++ b/database_ready_final (Marine Parade).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcus/Desktop/podsee centralised search engine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02BCC745-F9A1-F24B-B56E-674E611E64F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24454C21-B2C4-5B43-89DF-07F40668A0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="13620" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="offerings" sheetId="1" r:id="rId1"/>
@@ -1584,7 +1584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1281" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A501" zoomScale="82" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="A693" sqref="A693"/>
     </sheetView>
   </sheetViews>
@@ -23104,8 +23104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>